<commit_message>
Update Analyst rating changes.xlsx
</commit_message>
<xml_diff>
--- a/Analyst rating changes.xlsx
+++ b/Analyst rating changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/115e5277c8eb1d13/Documents/GitHub/Analyst-sentiment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="136" documentId="13_ncr:1_{50EA8B96-A233-42DC-AC20-99E1B30845A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66A5CE83-844A-4578-9EAF-5AFEBC43225A}"/>
+  <xr:revisionPtr revIDLastSave="186" documentId="13_ncr:1_{50EA8B96-A233-42DC-AC20-99E1B30845A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98545585-8B84-4965-8A9B-75844AB092A3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="131">
   <si>
     <t>Name</t>
   </si>
@@ -418,6 +418,12 @@
   </si>
   <si>
     <t>MEKKO</t>
+  </si>
+  <si>
+    <t>LUND B</t>
+  </si>
+  <si>
+    <t>IMP A SDB</t>
   </si>
 </sst>
 </file>
@@ -770,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8971C20D-DE11-9641-971F-C3D4179070FE}">
-  <dimension ref="A1:G129"/>
+  <dimension ref="A1:G135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,148 +814,142 @@
     </row>
     <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>44524</v>
+        <v>44525</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>130</v>
+      </c>
+      <c r="G2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>44525</v>
+      </c>
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>155</v>
+      </c>
+      <c r="G3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>44525</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2">
-        <v>965.2</v>
-      </c>
-      <c r="G2">
-        <v>822.96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>44524</v>
-      </c>
-      <c r="B3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <v>53.34</v>
-      </c>
-      <c r="G3">
-        <v>55.88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>44524</v>
-      </c>
-      <c r="B4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F4">
-        <v>162.56</v>
+        <v>285</v>
       </c>
       <c r="G4">
-        <v>166.624</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>44524</v>
+        <v>44525</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="D5">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="F5">
-        <v>310</v>
+        <v>155</v>
       </c>
       <c r="G5">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>44524</v>
+        <v>44525</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
       </c>
       <c r="F6">
-        <v>105</v>
-      </c>
-      <c r="G6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>44524</v>
+        <v>44525</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
       <c r="F7">
-        <v>274</v>
-      </c>
-      <c r="G7">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44524</v>
       </c>
       <c r="B8" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -958,13 +958,13 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F8">
-        <v>97</v>
+        <v>965.2</v>
       </c>
       <c r="G8">
-        <v>87</v>
+        <v>822.96</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,22 +972,22 @@
         <v>44524</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C9" t="s">
-        <v>120</v>
+        <v>44</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F9">
-        <v>340</v>
+        <v>53.34</v>
       </c>
       <c r="G9">
-        <v>270</v>
+        <v>55.88</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -995,22 +995,22 @@
         <v>44524</v>
       </c>
       <c r="B10" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C10" t="s">
-        <v>120</v>
+        <v>23</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
       </c>
       <c r="F10">
-        <v>185</v>
+        <v>162.56</v>
       </c>
       <c r="G10">
-        <v>150</v>
+        <v>166.624</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1018,239 +1018,242 @@
         <v>44524</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="F11">
-        <v>435</v>
+        <v>310</v>
       </c>
       <c r="G11">
-        <v>370</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>105</v>
+      </c>
+      <c r="G12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>274</v>
+      </c>
+      <c r="G13">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14">
+        <v>97</v>
+      </c>
+      <c r="G14">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15">
+        <v>340</v>
+      </c>
+      <c r="G15">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16">
+        <v>185</v>
+      </c>
+      <c r="G16">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <v>435</v>
+      </c>
+      <c r="G17">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>44523</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B18" t="s">
         <v>118</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C18" t="s">
         <v>119</v>
       </c>
-      <c r="D12">
+      <c r="D18">
         <v>-1</v>
       </c>
-      <c r="E12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12">
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18">
         <f>10.5*7.08</f>
         <v>74.34</v>
       </c>
-      <c r="G12">
+      <c r="G18">
         <f>12.5*7.08</f>
         <v>88.5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>44523</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B19" t="s">
         <v>26</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C19" t="s">
         <v>17</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13">
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19">
         <v>477</v>
       </c>
-      <c r="G13">
+      <c r="G19">
         <v>483</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>44523</v>
-      </c>
-      <c r="B14" t="s">
-        <v>117</v>
-      </c>
-      <c r="C14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14">
-        <v>128</v>
-      </c>
-      <c r="G14">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>44523</v>
-      </c>
-      <c r="B15" t="s">
-        <v>116</v>
-      </c>
-      <c r="C15" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15">
-        <v>100</v>
-      </c>
-      <c r="G15">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>44523</v>
-      </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" t="s">
-        <v>94</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16">
-        <v>82</v>
-      </c>
-      <c r="G16">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>44523</v>
-      </c>
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17">
-        <v>310</v>
-      </c>
-      <c r="G17">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>44522</v>
-      </c>
-      <c r="B18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" t="s">
-        <v>115</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18">
-        <v>370</v>
-      </c>
-      <c r="G18">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>44522</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19">
-        <v>1145.7</v>
-      </c>
-      <c r="G19">
-        <v>1181.8800000000001</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>44522</v>
+        <v>44523</v>
       </c>
       <c r="B20" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
       </c>
       <c r="F20">
-        <v>35</v>
+        <v>128</v>
+      </c>
+      <c r="G20">
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>44522</v>
+        <v>44523</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1259,21 +1262,21 @@
         <v>5</v>
       </c>
       <c r="F21">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="G21">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>44522</v>
+        <v>44523</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1282,61 +1285,67 @@
         <v>8</v>
       </c>
       <c r="F22">
-        <v>200</v>
+        <v>82</v>
       </c>
       <c r="G22">
-        <v>185</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>44519</v>
+        <v>44523</v>
       </c>
       <c r="B23" t="s">
-        <v>110</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D23">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="F23">
+        <v>310</v>
+      </c>
+      <c r="G23">
+        <v>300</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>44519</v>
+        <v>44522</v>
       </c>
       <c r="B24" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
+        <v>115</v>
       </c>
       <c r="D24">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F24">
-        <v>500</v>
+        <v>370</v>
       </c>
       <c r="G24">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>44519</v>
+        <v>44522</v>
       </c>
       <c r="B25" t="s">
-        <v>107</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1345,64 +1354,61 @@
         <v>8</v>
       </c>
       <c r="F25">
-        <v>170</v>
+        <v>1145.7</v>
       </c>
       <c r="G25">
-        <v>160</v>
+        <v>1181.8800000000001</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>44519</v>
+        <v>44522</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F26">
-        <v>147</v>
-      </c>
-      <c r="G26">
-        <v>140</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>44519</v>
+        <v>44522</v>
       </c>
       <c r="B27" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F27">
-        <v>199</v>
+        <v>126</v>
       </c>
       <c r="G27">
-        <v>190</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>44518</v>
+        <v>44522</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="C28" t="s">
         <v>12</v>
@@ -1414,67 +1420,61 @@
         <v>8</v>
       </c>
       <c r="F28">
-        <v>157</v>
+        <v>200</v>
       </c>
       <c r="G28">
-        <v>137</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>44518</v>
+        <v>44519</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>110</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E29" t="s">
         <v>5</v>
-      </c>
-      <c r="F29">
-        <v>125</v>
-      </c>
-      <c r="G29">
-        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>44518</v>
+        <v>44519</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
+        <v>106</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E30" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F30">
-        <v>142</v>
+        <v>500</v>
       </c>
       <c r="G30">
-        <v>160.5</v>
+        <v>540</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>44518</v>
+        <v>44519</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>107</v>
       </c>
       <c r="C31" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -1483,156 +1483,165 @@
         <v>8</v>
       </c>
       <c r="F31">
-        <v>483</v>
+        <v>170</v>
       </c>
       <c r="G31">
-        <v>471</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>44518</v>
+        <v>44519</v>
       </c>
       <c r="B32" t="s">
-        <v>25</v>
+        <v>108</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32" t="s">
         <v>8</v>
+      </c>
+      <c r="F32">
+        <v>147</v>
+      </c>
+      <c r="G32">
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>44517</v>
+        <v>44519</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
       <c r="C33" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D33">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F33">
-        <v>72</v>
+        <v>199</v>
       </c>
       <c r="G33">
-        <v>87</v>
+        <v>190</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>44517</v>
+        <v>44518</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D34">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F34">
-        <v>1050</v>
+        <v>157</v>
+      </c>
+      <c r="G34">
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>44517</v>
+        <v>44518</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F35">
-        <v>1100</v>
+        <v>125</v>
       </c>
       <c r="G35">
-        <v>990</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>44517</v>
+        <v>44518</v>
       </c>
       <c r="B36" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F36">
-        <v>261</v>
+        <v>142</v>
+      </c>
+      <c r="G36">
+        <v>160.5</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>44517</v>
+        <v>44518</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37" t="s">
         <v>8</v>
       </c>
       <c r="F37">
-        <v>155</v>
+        <v>483</v>
+      </c>
+      <c r="G37">
+        <v>471</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>44517</v>
+        <v>44518</v>
       </c>
       <c r="B38" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C38" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>5</v>
-      </c>
-      <c r="F38">
-        <v>145</v>
-      </c>
-      <c r="G38">
-        <v>136</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1640,22 +1649,22 @@
         <v>44517</v>
       </c>
       <c r="B39" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E39" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F39">
-        <v>327</v>
+        <v>72</v>
       </c>
       <c r="G39">
-        <v>320</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1663,22 +1672,19 @@
         <v>44517</v>
       </c>
       <c r="B40" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C40" t="s">
         <v>11</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F40">
-        <v>87</v>
-      </c>
-      <c r="G40">
-        <v>96</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1686,10 +1692,10 @@
         <v>44517</v>
       </c>
       <c r="B41" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -1698,182 +1704,176 @@
         <v>8</v>
       </c>
       <c r="F41">
-        <v>150</v>
+        <v>1100</v>
       </c>
       <c r="G41">
-        <v>180</v>
+        <v>990</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>44516</v>
+        <v>44517</v>
       </c>
       <c r="B42" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C42" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F42">
-        <v>1145</v>
-      </c>
-      <c r="G42">
-        <v>1160</v>
+        <v>261</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>44516</v>
+        <v>44517</v>
       </c>
       <c r="B43" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C43" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F43">
-        <v>118</v>
-      </c>
-      <c r="G43">
-        <v>123</v>
+        <v>155</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>44516</v>
+        <v>44517</v>
       </c>
       <c r="B44" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F44">
-        <v>380</v>
+        <v>145</v>
       </c>
       <c r="G44">
-        <v>357</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>44516</v>
+        <v>44517</v>
       </c>
       <c r="B45" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="C45" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D45">
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F45">
-        <v>685</v>
+        <v>327</v>
       </c>
       <c r="G45">
-        <v>558</v>
+        <v>320</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>44515</v>
+        <v>44517</v>
       </c>
       <c r="B46" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C46" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46" t="s">
         <v>8</v>
       </c>
       <c r="F46">
-        <v>165</v>
+        <v>87</v>
       </c>
       <c r="G46">
-        <v>165</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>44515</v>
+        <v>44517</v>
       </c>
       <c r="B47" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C47" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D47">
         <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="F47">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="G47">
-        <v>117</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>44515</v>
+        <v>44516</v>
       </c>
       <c r="B48" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C48" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F48">
-        <v>136</v>
+        <v>1145</v>
       </c>
       <c r="G48">
-        <v>180</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>44515</v>
+        <v>44516</v>
       </c>
       <c r="B49" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C49" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -1882,21 +1882,21 @@
         <v>5</v>
       </c>
       <c r="F49">
-        <v>2.7</v>
+        <v>118</v>
       </c>
       <c r="G49">
-        <v>2.8</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>44515</v>
+        <v>44516</v>
       </c>
       <c r="B50" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C50" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -1905,18 +1905,18 @@
         <v>8</v>
       </c>
       <c r="F50">
-        <v>70</v>
+        <v>380</v>
       </c>
       <c r="G50">
-        <v>54</v>
+        <v>357</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>44515</v>
+        <v>44516</v>
       </c>
       <c r="B51" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C51" t="s">
         <v>21</v>
@@ -1928,10 +1928,10 @@
         <v>5</v>
       </c>
       <c r="F51">
-        <v>228</v>
+        <v>685</v>
       </c>
       <c r="G51">
-        <v>206</v>
+        <v>558</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -1939,22 +1939,22 @@
         <v>44515</v>
       </c>
       <c r="B52" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C52" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E52" t="s">
         <v>8</v>
       </c>
       <c r="F52">
-        <v>16</v>
+        <v>165</v>
       </c>
       <c r="G52">
-        <v>17</v>
+        <v>165</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -1962,22 +1962,22 @@
         <v>44515</v>
       </c>
       <c r="B53" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C53" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D53">
         <v>0</v>
       </c>
       <c r="E53" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="F53">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="G53">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1985,16 +1985,22 @@
         <v>44515</v>
       </c>
       <c r="B54" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="C54" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="F54">
+        <v>136</v>
+      </c>
+      <c r="G54">
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2002,10 +2008,10 @@
         <v>44515</v>
       </c>
       <c r="B55" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C55" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -2014,10 +2020,10 @@
         <v>5</v>
       </c>
       <c r="F55">
-        <v>960</v>
+        <v>2.7</v>
       </c>
       <c r="G55">
-        <v>800</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2025,10 +2031,10 @@
         <v>44515</v>
       </c>
       <c r="B56" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C56" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -2037,10 +2043,10 @@
         <v>8</v>
       </c>
       <c r="F56">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="G56">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2048,22 +2054,22 @@
         <v>44515</v>
       </c>
       <c r="B57" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C57" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="D57">
         <v>0</v>
       </c>
       <c r="E57" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F57">
-        <v>51</v>
+        <v>228</v>
       </c>
       <c r="G57">
-        <v>65</v>
+        <v>206</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2071,10 +2077,10 @@
         <v>44515</v>
       </c>
       <c r="B58" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C58" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -2083,10 +2089,10 @@
         <v>8</v>
       </c>
       <c r="F58">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G58">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2094,79 +2100,73 @@
         <v>44515</v>
       </c>
       <c r="B59" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="C59" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E59" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F59">
-        <v>145</v>
+        <v>103</v>
       </c>
       <c r="G59">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>44512</v>
+        <v>44515</v>
       </c>
       <c r="B60" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C60" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60" t="s">
         <v>8</v>
-      </c>
-      <c r="F60">
-        <v>155</v>
-      </c>
-      <c r="G60">
-        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>44512</v>
+        <v>44515</v>
       </c>
       <c r="B61" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C61" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="D61">
         <v>0</v>
       </c>
       <c r="E61" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F61">
-        <v>90</v>
+        <v>960</v>
       </c>
       <c r="G61">
-        <v>85</v>
+        <v>800</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>44512</v>
+        <v>44515</v>
       </c>
       <c r="B62" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C62" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -2175,21 +2175,21 @@
         <v>8</v>
       </c>
       <c r="F62">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="G62">
-        <v>85</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>44512</v>
+        <v>44515</v>
       </c>
       <c r="B63" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C63" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -2198,56 +2198,56 @@
         <v>8</v>
       </c>
       <c r="F63">
-        <v>697</v>
+        <v>51</v>
       </c>
       <c r="G63">
-        <v>640</v>
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>44512</v>
+        <v>44515</v>
       </c>
       <c r="B64" t="s">
+        <v>46</v>
+      </c>
+      <c r="C64" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64">
         <v>32</v>
       </c>
-      <c r="C64" t="s">
-        <v>44</v>
-      </c>
-      <c r="D64">
-        <v>0</v>
-      </c>
-      <c r="E64" t="s">
-        <v>8</v>
-      </c>
-      <c r="F64">
-        <v>197</v>
-      </c>
       <c r="G64">
-        <v>185</v>
+        <v>37</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>44512</v>
+        <v>44515</v>
       </c>
       <c r="B65" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C65" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F65">
-        <v>235</v>
+        <v>145</v>
       </c>
       <c r="G65">
-        <v>220</v>
+        <v>120</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2255,22 +2255,22 @@
         <v>44512</v>
       </c>
       <c r="B66" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C66" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="D66">
         <v>0</v>
       </c>
       <c r="E66" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F66">
-        <v>215</v>
+        <v>155</v>
       </c>
       <c r="G66">
-        <v>205</v>
+        <v>145</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -2278,10 +2278,10 @@
         <v>44512</v>
       </c>
       <c r="B67" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C67" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -2290,64 +2290,67 @@
         <v>8</v>
       </c>
       <c r="F67">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="G67">
-        <v>28</v>
+        <v>85</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>44511</v>
+        <v>44512</v>
       </c>
       <c r="B68" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C68" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E68" t="s">
         <v>8</v>
       </c>
       <c r="F68">
-        <v>340</v>
+        <v>90</v>
       </c>
       <c r="G68">
-        <v>295</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>44511</v>
+        <v>44512</v>
       </c>
       <c r="B69" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C69" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D69">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E69" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="F69">
-        <v>310</v>
+        <v>697</v>
+      </c>
+      <c r="G69">
+        <v>640</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>44511</v>
+        <v>44512</v>
       </c>
       <c r="B70" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="C70" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -2356,133 +2359,130 @@
         <v>8</v>
       </c>
       <c r="F70">
-        <v>360</v>
+        <v>197</v>
       </c>
       <c r="G70">
-        <v>320</v>
+        <v>185</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>44511</v>
+        <v>44512</v>
       </c>
       <c r="B71" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C71" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="D71">
         <v>0</v>
       </c>
       <c r="E71" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F71">
-        <v>990</v>
+        <v>235</v>
       </c>
       <c r="G71">
-        <v>930</v>
+        <v>220</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>44511</v>
+        <v>44512</v>
       </c>
       <c r="B72" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="C72" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="D72">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E72" t="s">
         <v>5</v>
       </c>
       <c r="F72">
-        <v>75</v>
+        <v>215</v>
       </c>
       <c r="G72">
-        <v>145</v>
+        <v>205</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>44510</v>
+        <v>44512</v>
       </c>
       <c r="B73" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C73" t="s">
+        <v>44</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73" t="s">
+        <v>8</v>
+      </c>
+      <c r="F73">
         <v>31</v>
       </c>
-      <c r="D73">
-        <v>0</v>
-      </c>
-      <c r="E73" t="s">
-        <v>5</v>
-      </c>
-      <c r="F73">
-        <v>51</v>
-      </c>
       <c r="G73">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>44510</v>
+        <v>44511</v>
       </c>
       <c r="B74" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C74" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F74">
-        <v>325</v>
+        <v>340</v>
       </c>
       <c r="G74">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>44510</v>
+        <v>44511</v>
       </c>
       <c r="B75" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C75" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D75">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E75" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="F75">
-        <v>175</v>
-      </c>
-      <c r="G75">
-        <v>190</v>
+        <v>310</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>44510</v>
+        <v>44511</v>
       </c>
       <c r="B76" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C76" t="s">
         <v>21</v>
@@ -2494,18 +2494,18 @@
         <v>8</v>
       </c>
       <c r="F76">
-        <v>32</v>
+        <v>360</v>
       </c>
       <c r="G76">
-        <v>30</v>
+        <v>320</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>44510</v>
+        <v>44511</v>
       </c>
       <c r="B77" t="s">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="C77" t="s">
         <v>12</v>
@@ -2517,21 +2517,21 @@
         <v>8</v>
       </c>
       <c r="F77">
-        <v>497</v>
+        <v>990</v>
       </c>
       <c r="G77">
-        <v>512</v>
+        <v>930</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>44510</v>
+        <v>44511</v>
       </c>
       <c r="B78" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C78" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D78">
         <v>-1</v>
@@ -2540,10 +2540,10 @@
         <v>5</v>
       </c>
       <c r="F78">
-        <v>360</v>
+        <v>75</v>
       </c>
       <c r="G78">
-        <v>340</v>
+        <v>145</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -2551,22 +2551,22 @@
         <v>44510</v>
       </c>
       <c r="B79" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C79" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="D79">
         <v>0</v>
       </c>
       <c r="E79" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F79">
-        <v>92.5</v>
+        <v>51</v>
       </c>
       <c r="G79">
-        <v>83</v>
+        <v>45</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -2574,7 +2574,7 @@
         <v>44510</v>
       </c>
       <c r="B80" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C80" t="s">
         <v>45</v>
@@ -2583,13 +2583,13 @@
         <v>0</v>
       </c>
       <c r="E80" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F80">
-        <v>100</v>
+        <v>325</v>
       </c>
       <c r="G80">
-        <v>89</v>
+        <v>300</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -2597,22 +2597,22 @@
         <v>44510</v>
       </c>
       <c r="B81" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="C81" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="D81">
         <v>0</v>
       </c>
       <c r="E81" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F81">
-        <v>139</v>
+        <v>175</v>
       </c>
       <c r="G81">
-        <v>175</v>
+        <v>190</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -2620,10 +2620,10 @@
         <v>44510</v>
       </c>
       <c r="B82" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C82" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -2632,10 +2632,10 @@
         <v>8</v>
       </c>
       <c r="F82">
-        <v>190</v>
+        <v>32</v>
       </c>
       <c r="G82">
-        <v>140</v>
+        <v>30</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -2643,10 +2643,10 @@
         <v>44510</v>
       </c>
       <c r="B83" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C83" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -2655,84 +2655,87 @@
         <v>8</v>
       </c>
       <c r="F83">
-        <v>160</v>
+        <v>497</v>
       </c>
       <c r="G83">
-        <v>140</v>
+        <v>512</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>44509</v>
+        <v>44510</v>
       </c>
       <c r="B84" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C84" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="D84">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E84" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F84">
-        <v>240</v>
+        <v>360</v>
+      </c>
+      <c r="G84">
+        <v>340</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>44509</v>
+        <v>44510</v>
       </c>
       <c r="B85" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C85" t="s">
         <v>11</v>
       </c>
       <c r="D85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E85" t="s">
         <v>8</v>
       </c>
       <c r="F85">
-        <v>211</v>
+        <v>92.5</v>
       </c>
       <c r="G85">
-        <v>222</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>44509</v>
+        <v>44510</v>
       </c>
       <c r="B86" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C86" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D86">
         <v>0</v>
       </c>
       <c r="E86" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="F86">
-        <v>248</v>
+        <v>100</v>
       </c>
       <c r="G86">
-        <v>231</v>
+        <v>89</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>44509</v>
+        <v>44510</v>
       </c>
       <c r="B87" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="C87" t="s">
         <v>11</v>
@@ -2741,24 +2744,24 @@
         <v>0</v>
       </c>
       <c r="E87" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F87">
-        <v>575</v>
+        <v>139</v>
       </c>
       <c r="G87">
-        <v>545</v>
+        <v>175</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>44509</v>
+        <v>44510</v>
       </c>
       <c r="B88" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C88" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -2767,110 +2770,110 @@
         <v>8</v>
       </c>
       <c r="F88">
-        <v>328</v>
+        <v>190</v>
       </c>
       <c r="G88">
-        <v>310</v>
+        <v>140</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>44505</v>
+        <v>44510</v>
       </c>
       <c r="B89" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="C89" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="D89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E89" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F89">
-        <v>170</v>
+        <v>160</v>
+      </c>
+      <c r="G89">
+        <v>140</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>44505</v>
+        <v>44509</v>
       </c>
       <c r="B90" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C90" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="D90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E90" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="F90">
-        <v>180</v>
-      </c>
-      <c r="G90">
-        <v>175</v>
+        <v>240</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>44505</v>
+        <v>44509</v>
       </c>
       <c r="B91" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C91" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F91">
-        <v>55</v>
+        <v>211</v>
       </c>
       <c r="G91">
-        <v>40</v>
+        <v>222</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>44505</v>
+        <v>44509</v>
       </c>
       <c r="B92" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="C92" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="D92">
         <v>0</v>
       </c>
       <c r="E92" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="F92">
-        <v>67</v>
+        <v>248</v>
       </c>
       <c r="G92">
-        <v>46</v>
+        <v>231</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>44505</v>
+        <v>44509</v>
       </c>
       <c r="B93" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="C93" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -2879,21 +2882,21 @@
         <v>8</v>
       </c>
       <c r="F93">
-        <v>66</v>
+        <v>575</v>
       </c>
       <c r="G93">
-        <v>60</v>
+        <v>545</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>44505</v>
+        <v>44509</v>
       </c>
       <c r="B94" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="C94" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -2902,10 +2905,10 @@
         <v>8</v>
       </c>
       <c r="F94">
-        <v>68</v>
+        <v>328</v>
       </c>
       <c r="G94">
-        <v>55</v>
+        <v>310</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -2913,22 +2916,19 @@
         <v>44505</v>
       </c>
       <c r="B95" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C95" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="D95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E95" t="s">
         <v>5</v>
       </c>
       <c r="F95">
-        <v>60</v>
-      </c>
-      <c r="G95">
-        <v>50</v>
+        <v>170</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -2936,22 +2936,22 @@
         <v>44505</v>
       </c>
       <c r="B96" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C96" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D96">
         <v>0</v>
       </c>
       <c r="E96" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="F96">
-        <v>210</v>
+        <v>180</v>
       </c>
       <c r="G96">
-        <v>200</v>
+        <v>175</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -2959,7 +2959,7 @@
         <v>44505</v>
       </c>
       <c r="B97" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="C97" t="s">
         <v>23</v>
@@ -2971,10 +2971,10 @@
         <v>5</v>
       </c>
       <c r="F97">
-        <v>130</v>
+        <v>55</v>
       </c>
       <c r="G97">
-        <v>110</v>
+        <v>40</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -2982,22 +2982,22 @@
         <v>44505</v>
       </c>
       <c r="B98" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="C98" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="D98">
         <v>0</v>
       </c>
       <c r="E98" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F98">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="G98">
-        <v>111</v>
+        <v>46</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -3005,10 +3005,10 @@
         <v>44505</v>
       </c>
       <c r="B99" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C99" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -3017,41 +3017,44 @@
         <v>8</v>
       </c>
       <c r="F99">
-        <v>275</v>
+        <v>66</v>
       </c>
       <c r="G99">
-        <v>300</v>
+        <v>60</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>44504</v>
+        <v>44505</v>
       </c>
       <c r="B100" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="C100" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="D100">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E100" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="F100">
-        <v>123</v>
+        <v>68</v>
+      </c>
+      <c r="G100">
+        <v>55</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>44504</v>
+        <v>44505</v>
       </c>
       <c r="B101" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="C101" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -3060,41 +3063,41 @@
         <v>5</v>
       </c>
       <c r="F101">
-        <v>115</v>
+        <v>60</v>
       </c>
       <c r="G101">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>44504</v>
+        <v>44505</v>
       </c>
       <c r="B102" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C102" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D102">
         <v>0</v>
       </c>
       <c r="E102" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F102">
-        <v>350</v>
+        <v>210</v>
       </c>
       <c r="G102">
-        <v>245</v>
+        <v>200</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>44504</v>
+        <v>44505</v>
       </c>
       <c r="B103" t="s">
-        <v>82</v>
+        <v>28</v>
       </c>
       <c r="C103" t="s">
         <v>23</v>
@@ -3106,41 +3109,44 @@
         <v>5</v>
       </c>
       <c r="F103">
-        <v>281</v>
+        <v>130</v>
       </c>
       <c r="G103">
-        <v>270</v>
+        <v>110</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>44503</v>
+        <v>44505</v>
       </c>
       <c r="B104" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="C104" t="s">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="D104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E104" t="s">
         <v>5</v>
       </c>
       <c r="F104">
-        <v>272</v>
+        <v>120</v>
+      </c>
+      <c r="G104">
+        <v>111</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>44503</v>
+        <v>44505</v>
       </c>
       <c r="B105" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C105" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="D105">
         <v>0</v>
@@ -3149,90 +3155,87 @@
         <v>8</v>
       </c>
       <c r="F105">
-        <v>95</v>
+        <v>275</v>
       </c>
       <c r="G105">
-        <v>100</v>
+        <v>300</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>44503</v>
+        <v>44504</v>
       </c>
       <c r="B106" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C106" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="D106">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E106" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="F106">
-        <v>180</v>
-      </c>
-      <c r="G106">
-        <v>176</v>
+        <v>123</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>44503</v>
+        <v>44504</v>
       </c>
       <c r="B107" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C107" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D107">
         <v>0</v>
       </c>
       <c r="E107" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F107">
-        <v>290</v>
+        <v>115</v>
       </c>
       <c r="G107">
-        <v>270</v>
+        <v>100</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>44503</v>
+        <v>44504</v>
       </c>
       <c r="B108" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C108" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D108">
         <v>0</v>
       </c>
       <c r="E108" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="F108">
-        <v>130</v>
+        <v>350</v>
       </c>
       <c r="G108">
-        <v>125</v>
+        <v>245</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>44503</v>
+        <v>44504</v>
       </c>
       <c r="B109" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C109" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="D109">
         <v>0</v>
@@ -3241,10 +3244,10 @@
         <v>5</v>
       </c>
       <c r="F109">
-        <v>135</v>
+        <v>281</v>
       </c>
       <c r="G109">
-        <v>130</v>
+        <v>270</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -3252,22 +3255,19 @@
         <v>44503</v>
       </c>
       <c r="B110" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C110" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="D110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E110" t="s">
-        <v>90</v>
+        <v>5</v>
       </c>
       <c r="F110">
-        <v>123</v>
-      </c>
-      <c r="G110">
-        <v>120</v>
+        <v>272</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -3275,22 +3275,22 @@
         <v>44503</v>
       </c>
       <c r="B111" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C111" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="D111">
         <v>0</v>
       </c>
       <c r="E111" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F111">
-        <v>540</v>
+        <v>95</v>
       </c>
       <c r="G111">
-        <v>530</v>
+        <v>100</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -3298,10 +3298,10 @@
         <v>44503</v>
       </c>
       <c r="B112" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="C112" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="D112">
         <v>0</v>
@@ -3310,133 +3310,136 @@
         <v>8</v>
       </c>
       <c r="F112">
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="G112">
-        <v>163</v>
+        <v>176</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>44502</v>
+        <v>44503</v>
       </c>
       <c r="B113" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C113" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D113">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E113" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="F113">
-        <v>59</v>
+        <v>290</v>
+      </c>
+      <c r="G113">
+        <v>270</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>44502</v>
+        <v>44503</v>
       </c>
       <c r="B114" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C114" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="D114">
         <v>0</v>
       </c>
       <c r="E114" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="F114">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="G114">
-        <v>80</v>
+        <v>125</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>44502</v>
+        <v>44503</v>
       </c>
       <c r="B115" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C115" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="D115">
         <v>0</v>
       </c>
       <c r="E115" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F115">
-        <v>88</v>
+        <v>135</v>
       </c>
       <c r="G115">
-        <v>91</v>
+        <v>130</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>44502</v>
+        <v>44503</v>
       </c>
       <c r="B116" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C116" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="D116">
         <v>0</v>
       </c>
       <c r="E116" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="F116">
-        <v>54</v>
+        <v>123</v>
       </c>
       <c r="G116">
-        <v>46</v>
+        <v>120</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>44502</v>
+        <v>44503</v>
       </c>
       <c r="B117" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C117" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="D117">
         <v>0</v>
       </c>
       <c r="E117" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F117">
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="G117">
-        <v>540</v>
+        <v>530</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>44502</v>
+        <v>44503</v>
       </c>
       <c r="B118" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="C118" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D118">
         <v>0</v>
@@ -3445,41 +3448,41 @@
         <v>8</v>
       </c>
       <c r="F118">
-        <v>810</v>
+        <v>140</v>
       </c>
       <c r="G118">
-        <v>760</v>
+        <v>163</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>44501</v>
+        <v>44502</v>
       </c>
       <c r="B119" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="C119" t="s">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="D119">
         <v>-1</v>
       </c>
       <c r="E119" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="F119">
-        <v>360</v>
+        <v>59</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>44501</v>
+        <v>44502</v>
       </c>
       <c r="B120" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C120" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D120">
         <v>0</v>
@@ -3488,87 +3491,90 @@
         <v>8</v>
       </c>
       <c r="F120">
-        <v>208</v>
+        <v>75</v>
       </c>
       <c r="G120">
-        <v>206</v>
+        <v>80</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>44501</v>
+        <v>44502</v>
       </c>
       <c r="B121" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C121" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E121" t="s">
         <v>8</v>
       </c>
       <c r="F121">
-        <v>151</v>
+        <v>88</v>
+      </c>
+      <c r="G121">
+        <v>91</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>44501</v>
+        <v>44502</v>
       </c>
       <c r="B122" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C122" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="D122">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="E122" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="F122">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="G122">
-        <v>208</v>
+        <v>46</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>44501</v>
+        <v>44502</v>
       </c>
       <c r="B123" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C123" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D123">
         <v>0</v>
       </c>
       <c r="E123" t="s">
-        <v>90</v>
+        <v>8</v>
       </c>
       <c r="F123">
-        <v>204</v>
+        <v>550</v>
       </c>
       <c r="G123">
-        <v>192</v>
+        <v>540</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>44501</v>
+        <v>44502</v>
       </c>
       <c r="B124" t="s">
-        <v>101</v>
+        <v>42</v>
       </c>
       <c r="C124" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D124">
         <v>0</v>
@@ -3577,10 +3583,10 @@
         <v>8</v>
       </c>
       <c r="F124">
-        <v>175</v>
+        <v>810</v>
       </c>
       <c r="G124">
-        <v>192</v>
+        <v>760</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -3588,22 +3594,19 @@
         <v>44501</v>
       </c>
       <c r="B125" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="C125" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="D125">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E125" t="s">
-        <v>90</v>
+        <v>5</v>
       </c>
       <c r="F125">
-        <v>146</v>
-      </c>
-      <c r="G125">
-        <v>135</v>
+        <v>360</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -3611,22 +3614,22 @@
         <v>44501</v>
       </c>
       <c r="B126" t="s">
-        <v>4</v>
+        <v>98</v>
       </c>
       <c r="C126" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="D126">
         <v>0</v>
       </c>
       <c r="E126" t="s">
-        <v>90</v>
+        <v>8</v>
       </c>
       <c r="F126">
-        <v>88</v>
+        <v>208</v>
       </c>
       <c r="G126">
-        <v>85</v>
+        <v>206</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -3634,22 +3637,19 @@
         <v>44501</v>
       </c>
       <c r="B127" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C127" t="s">
         <v>23</v>
       </c>
       <c r="D127">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E127" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F127">
-        <v>85</v>
-      </c>
-      <c r="G127">
-        <v>100</v>
+        <v>151</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -3657,22 +3657,22 @@
         <v>44501</v>
       </c>
       <c r="B128" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C128" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D128">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="E128" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="F128">
-        <v>210</v>
+        <v>105</v>
       </c>
       <c r="G128">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -3680,21 +3680,159 @@
         <v>44501</v>
       </c>
       <c r="B129" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C129" t="s">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="D129">
         <v>0</v>
       </c>
       <c r="E129" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="F129">
         <v>204</v>
       </c>
       <c r="G129">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B130" t="s">
+        <v>101</v>
+      </c>
+      <c r="C130" t="s">
+        <v>21</v>
+      </c>
+      <c r="D130">
+        <v>0</v>
+      </c>
+      <c r="E130" t="s">
+        <v>8</v>
+      </c>
+      <c r="F130">
+        <v>175</v>
+      </c>
+      <c r="G130">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B131" t="s">
+        <v>81</v>
+      </c>
+      <c r="C131" t="s">
+        <v>54</v>
+      </c>
+      <c r="D131">
+        <v>0</v>
+      </c>
+      <c r="E131" t="s">
+        <v>90</v>
+      </c>
+      <c r="F131">
+        <v>146</v>
+      </c>
+      <c r="G131">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B132" t="s">
+        <v>4</v>
+      </c>
+      <c r="C132" t="s">
+        <v>54</v>
+      </c>
+      <c r="D132">
+        <v>0</v>
+      </c>
+      <c r="E132" t="s">
+        <v>90</v>
+      </c>
+      <c r="F132">
+        <v>88</v>
+      </c>
+      <c r="G132">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B133" t="s">
+        <v>102</v>
+      </c>
+      <c r="C133" t="s">
+        <v>23</v>
+      </c>
+      <c r="D133">
+        <v>0</v>
+      </c>
+      <c r="E133" t="s">
+        <v>5</v>
+      </c>
+      <c r="F133">
+        <v>85</v>
+      </c>
+      <c r="G133">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B134" t="s">
+        <v>103</v>
+      </c>
+      <c r="C134" t="s">
+        <v>23</v>
+      </c>
+      <c r="D134">
+        <v>0</v>
+      </c>
+      <c r="E134" t="s">
+        <v>8</v>
+      </c>
+      <c r="F134">
+        <v>210</v>
+      </c>
+      <c r="G134">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B135" t="s">
+        <v>104</v>
+      </c>
+      <c r="C135" t="s">
+        <v>105</v>
+      </c>
+      <c r="D135">
+        <v>0</v>
+      </c>
+      <c r="E135" t="s">
+        <v>5</v>
+      </c>
+      <c r="F135">
+        <v>204</v>
+      </c>
+      <c r="G135">
         <v>210</v>
       </c>
     </row>

</xml_diff>